<commit_message>
Restriccion de Jueces y TimeGrains funcionando
Se cargan las restricciones comunes (dia de la semana) y las restricciones especiales (fecha especifica) que se encuentran en formato XML.
</commit_message>
<xml_diff>
--- a/examples/sources/data/unsolved/2019-9-5.xlsx
+++ b/examples/sources/data/unsolved/2019-9-5.xlsx
@@ -8,74 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danilo Reitano\Documents\GitHub\optaplanner-time\examples\sources\data\unsolved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785F7DD0-B500-40B6-ADB4-185A913BC49D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEF19F9-EF8D-4AFF-854D-DC07C5FF2AA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Configuration" sheetId="2" r:id="rId1"/>
-    <sheet name="Audiencias" sheetId="9" r:id="rId2"/>
+    <sheet name="Audiencias" sheetId="9" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="129">
-  <si>
-    <t>Constraint</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Room conflict</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Start and end on same day</t>
-  </si>
-  <si>
-    <t>Don't go in overtime</t>
-  </si>
-  <si>
-    <t>Do not conflict Juez</t>
-  </si>
-  <si>
-    <t>Do not use room in prohibited time</t>
-  </si>
-  <si>
-    <t>Do not conflict Fiscal</t>
-  </si>
-  <si>
-    <t>Do not conflict Defensor</t>
-  </si>
-  <si>
-    <t>Respect Minimum Starting Time</t>
-  </si>
-  <si>
-    <t>Respect Maximum Starting Time</t>
-  </si>
-  <si>
-    <t>One TimeGrain break between two consecutive meetings</t>
-  </si>
-  <si>
-    <t>One TimeGrain Juez</t>
-  </si>
-  <si>
-    <t>One TimeGrain Defensor</t>
-  </si>
-  <si>
-    <t>One TimeGrain Fiscal</t>
-  </si>
-  <si>
-    <t>Do all meetings as soon as possible</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="110">
   <si>
     <t>Id</t>
   </si>
@@ -405,9 +350,6 @@
   </si>
   <si>
     <t>05-09-2019</t>
-  </si>
-  <si>
-    <t>Don't start after maximum starting time of the day</t>
   </si>
 </sst>
 </file>
@@ -417,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,###,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,20 +398,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -496,26 +425,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -792,204 +712,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6">
-        <v>100</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6">
-        <v>100</v>
-      </c>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6">
-        <v>100</v>
-      </c>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6">
-        <v>100</v>
-      </c>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1006,34 +734,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="10" t="s">
-        <v>127</v>
+      <c r="A1" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>106</v>
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -1046,7 +774,7 @@
         <v>99816</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1">
         <v>816</v>
@@ -1058,13 +786,13 @@
         <v>368</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1">
         <v>1072</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1077,7 +805,7 @@
         <v>99817</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1">
         <v>818</v>
@@ -1089,13 +817,13 @@
         <v>804</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>832</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1108,7 +836,7 @@
         <v>99818</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1">
         <v>817</v>
@@ -1120,13 +848,13 @@
         <v>323</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G5" s="1">
         <v>379</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1139,7 +867,7 @@
         <v>99820</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1">
         <v>821</v>
@@ -1151,13 +879,13 @@
         <v>412</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1">
         <v>872</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1170,7 +898,7 @@
         <v>99821</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1">
         <v>823</v>
@@ -1182,13 +910,13 @@
         <v>399</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1">
         <v>876</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1201,7 +929,7 @@
         <v>99822</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1">
         <v>827</v>
@@ -1213,13 +941,13 @@
         <v>323</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1">
         <v>703</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1232,7 +960,7 @@
         <v>99823</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1">
         <v>828</v>
@@ -1244,13 +972,13 @@
         <v>1096</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>511</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1263,7 +991,7 @@
         <v>99824</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C10" s="1">
         <v>854</v>
@@ -1275,13 +1003,13 @@
         <v>664</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G10" s="1">
         <v>643</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1294,7 +1022,7 @@
         <v>99825</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1">
         <v>827</v>
@@ -1306,13 +1034,13 @@
         <v>323</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1">
         <v>530</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1325,7 +1053,7 @@
         <v>99826</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1">
         <v>816</v>
@@ -1337,13 +1065,13 @@
         <v>1096</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1">
         <v>358</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1356,7 +1084,7 @@
         <v>99828</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1">
         <v>820</v>
@@ -1368,13 +1096,13 @@
         <v>795</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1">
         <v>835</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1387,7 +1115,7 @@
         <v>99829</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1">
         <v>820</v>
@@ -1399,13 +1127,13 @@
         <v>795</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1">
         <v>837</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1418,7 +1146,7 @@
         <v>99830</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1">
         <v>820</v>
@@ -1430,13 +1158,13 @@
         <v>407</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="G15" s="1">
         <v>453</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1449,7 +1177,7 @@
         <v>99831</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1">
         <v>820</v>
@@ -1461,13 +1189,13 @@
         <v>323</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1">
         <v>836</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1480,7 +1208,7 @@
         <v>99832</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C17" s="1">
         <v>820</v>
@@ -1492,13 +1220,13 @@
         <v>392</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1">
         <v>712</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1511,7 +1239,7 @@
         <v>99833</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1">
         <v>823</v>
@@ -1523,13 +1251,13 @@
         <v>804</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1">
         <v>540</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1542,7 +1270,7 @@
         <v>99834</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1">
         <v>823</v>
@@ -1554,13 +1282,13 @@
         <v>323</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G19" s="1">
         <v>387</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1573,7 +1301,7 @@
         <v>99836</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1">
         <v>823</v>
@@ -1585,13 +1313,13 @@
         <v>323</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="G20" s="1">
         <v>540</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1604,7 +1332,7 @@
         <v>99837</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1">
         <v>823</v>
@@ -1616,13 +1344,13 @@
         <v>802</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1">
         <v>832</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1635,7 +1363,7 @@
         <v>99838</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1">
         <v>816</v>
@@ -1647,13 +1375,13 @@
         <v>323</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G22" s="1">
         <v>377</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1666,7 +1394,7 @@
         <v>99839</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1">
         <v>823</v>
@@ -1678,13 +1406,13 @@
         <v>802</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1">
         <v>540</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1697,7 +1425,7 @@
         <v>99840</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1">
         <v>820</v>
@@ -1709,13 +1437,13 @@
         <v>571</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G24" s="1">
         <v>1231</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1728,7 +1456,7 @@
         <v>99841</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C25" s="1">
         <v>823</v>
@@ -1740,13 +1468,13 @@
         <v>802</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G25" s="1">
         <v>833</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1759,7 +1487,7 @@
         <v>99842</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1">
         <v>823</v>
@@ -1771,13 +1499,13 @@
         <v>360</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G26" s="1">
         <v>703</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1790,7 +1518,7 @@
         <v>99844</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1">
         <v>823</v>
@@ -1802,13 +1530,13 @@
         <v>407</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="G27" s="1">
         <v>732</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1821,7 +1549,7 @@
         <v>99846</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1">
         <v>823</v>
@@ -1833,13 +1561,13 @@
         <v>803</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G28" s="1">
         <v>540</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1852,7 +1580,7 @@
         <v>99849</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C29" s="1">
         <v>848</v>
@@ -1864,13 +1592,13 @@
         <v>407</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="G29" s="1">
         <v>378</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -1883,7 +1611,7 @@
         <v>99850</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1">
         <v>377</v>
@@ -1895,13 +1623,13 @@
         <v>398</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <v>485</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -1914,7 +1642,7 @@
         <v>99851</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1">
         <v>823</v>
@@ -1926,13 +1654,13 @@
         <v>553</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G31" s="1">
         <v>381</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1945,7 +1673,7 @@
         <v>99852</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1">
         <v>848</v>
@@ -1957,13 +1685,13 @@
         <v>804</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1">
         <v>835</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1976,7 +1704,7 @@
         <v>99853</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1">
         <v>823</v>
@@ -1988,13 +1716,13 @@
         <v>664</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G33" s="1">
         <v>647</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2007,7 +1735,7 @@
         <v>99854</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C34" s="1">
         <v>823</v>
@@ -2019,13 +1747,13 @@
         <v>396</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G34" s="1">
         <v>387</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2038,7 +1766,7 @@
         <v>99856</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1">
         <v>823</v>
@@ -2050,13 +1778,13 @@
         <v>562</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G35" s="1">
         <v>732</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2069,7 +1797,7 @@
         <v>99857</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C36" s="1">
         <v>828</v>
@@ -2081,13 +1809,13 @@
         <v>323</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G36" s="1">
         <v>704</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2100,7 +1828,7 @@
         <v>99858</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1">
         <v>821</v>
@@ -2112,13 +1840,13 @@
         <v>392</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G37" s="1">
         <v>383</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2131,7 +1859,7 @@
         <v>99859</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1">
         <v>848</v>
@@ -2143,13 +1871,13 @@
         <v>323</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="G38" s="1">
         <v>1175</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2162,7 +1890,7 @@
         <v>99860</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1">
         <v>823</v>
@@ -2174,13 +1902,13 @@
         <v>396</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G39" s="1">
         <v>703</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2193,7 +1921,7 @@
         <v>99861</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C40" s="1">
         <v>848</v>
@@ -2205,13 +1933,13 @@
         <v>323</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="G40" s="1">
         <v>1306</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2224,7 +1952,7 @@
         <v>99862</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C41" s="1">
         <v>828</v>
@@ -2236,13 +1964,13 @@
         <v>323</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="G41" s="1">
         <v>516</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2255,7 +1983,7 @@
         <v>99864</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1">
         <v>823</v>
@@ -2267,13 +1995,13 @@
         <v>11</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G42" s="1">
         <v>489</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2286,7 +2014,7 @@
         <v>99865</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C43" s="1">
         <v>863</v>
@@ -2298,13 +2026,13 @@
         <v>795</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G43" s="1">
         <v>847</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -2317,7 +2045,7 @@
         <v>99866</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C44" s="1">
         <v>820</v>
@@ -2329,13 +2057,13 @@
         <v>323</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="G44" s="1">
         <v>530</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -2348,7 +2076,7 @@
         <v>99867</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1">
         <v>848</v>
@@ -2360,13 +2088,13 @@
         <v>795</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G45" s="1">
         <v>825</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -2379,7 +2107,7 @@
         <v>99868</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1">
         <v>823</v>
@@ -2391,13 +2119,13 @@
         <v>368</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="G46" s="1">
         <v>380</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -2410,7 +2138,7 @@
         <v>99869</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1">
         <v>815</v>
@@ -2422,13 +2150,13 @@
         <v>323</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G47" s="1">
         <v>358</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -2441,7 +2169,7 @@
         <v>99870</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C48" s="1">
         <v>817</v>
@@ -2453,13 +2181,13 @@
         <v>323</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="G48" s="1">
         <v>379</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -2472,7 +2200,7 @@
         <v>99871</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C49" s="1">
         <v>820</v>
@@ -2484,13 +2212,13 @@
         <v>556</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G49" s="1">
         <v>527</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -2503,7 +2231,7 @@
         <v>99872</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C50" s="1">
         <v>827</v>
@@ -2515,13 +2243,13 @@
         <v>323</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G50" s="1">
         <v>843</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -2534,7 +2262,7 @@
         <v>99873</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C51" s="1">
         <v>823</v>
@@ -2546,13 +2274,13 @@
         <v>690</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G51" s="1">
         <v>1179</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -2565,7 +2293,7 @@
         <v>99875</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C52" s="1">
         <v>377</v>
@@ -2577,13 +2305,13 @@
         <v>398</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G52" s="1">
         <v>485</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -2596,7 +2324,7 @@
         <v>99876</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C53" s="1">
         <v>823</v>
@@ -2608,13 +2336,13 @@
         <v>362</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="G53" s="1">
         <v>874</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -2627,7 +2355,7 @@
         <v>99877</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C54" s="1">
         <v>828</v>
@@ -2639,13 +2367,13 @@
         <v>362</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="G54" s="1">
         <v>872</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -2658,7 +2386,7 @@
         <v>99878</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C55" s="1">
         <v>377</v>
@@ -2670,13 +2398,13 @@
         <v>398</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G55" s="1">
         <v>485</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -2689,7 +2417,7 @@
         <v>99879</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C56" s="1">
         <v>819</v>
@@ -2701,13 +2429,13 @@
         <v>562</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G56" s="1">
         <v>1072</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -2720,7 +2448,7 @@
         <v>99880</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C57" s="1">
         <v>823</v>
@@ -2732,13 +2460,13 @@
         <v>690</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G57" s="1">
         <v>849</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -2751,7 +2479,7 @@
         <v>99881</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C58" s="1">
         <v>377</v>
@@ -2763,13 +2491,13 @@
         <v>398</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G58" s="1">
         <v>494</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -2782,7 +2510,7 @@
         <v>99882</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C59" s="1">
         <v>377</v>
@@ -2794,13 +2522,13 @@
         <v>398</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G59" s="1">
         <v>485</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -2813,7 +2541,7 @@
         <v>99883</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C60" s="1">
         <v>377</v>
@@ -2825,13 +2553,13 @@
         <v>398</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G60" s="1">
         <v>485</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -2844,7 +2572,7 @@
         <v>99884</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C61" s="1">
         <v>828</v>
@@ -2856,13 +2584,13 @@
         <v>323</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G61" s="1">
         <v>1084</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -2875,7 +2603,7 @@
         <v>99885</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C62" s="1">
         <v>378</v>
@@ -2887,13 +2615,13 @@
         <v>398</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G62" s="1">
         <v>485</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -2906,7 +2634,7 @@
         <v>99886</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C63" s="1">
         <v>827</v>
@@ -2918,13 +2646,13 @@
         <v>323</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G63" s="1">
         <v>470</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -2937,7 +2665,7 @@
         <v>99887</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C64" s="1">
         <v>823</v>
@@ -2949,13 +2677,13 @@
         <v>693</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G64" s="1">
         <v>1179</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -2968,7 +2696,7 @@
         <v>99889</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C65" s="1">
         <v>819</v>
@@ -2980,13 +2708,13 @@
         <v>323</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G65" s="1">
         <v>541</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -2999,7 +2727,7 @@
         <v>99890</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C66" s="1">
         <v>822</v>
@@ -3011,13 +2739,13 @@
         <v>323</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="G66" s="1">
         <v>1086</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -3030,7 +2758,7 @@
         <v>99891</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C67" s="1">
         <v>823</v>
@@ -3042,13 +2770,13 @@
         <v>395</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G67" s="1">
         <v>489</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
@@ -3061,7 +2789,7 @@
         <v>99892</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C68" s="1">
         <v>823</v>
@@ -3073,13 +2801,13 @@
         <v>689</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="G68" s="1">
         <v>1180</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
@@ -3092,7 +2820,7 @@
         <v>99893</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C69" s="1">
         <v>828</v>
@@ -3104,13 +2832,13 @@
         <v>323</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="G69" s="1">
         <v>453</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -3123,7 +2851,7 @@
         <v>99894</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C70" s="1">
         <v>821</v>
@@ -3135,13 +2863,13 @@
         <v>553</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G70" s="1">
         <v>1210</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
@@ -3154,7 +2882,7 @@
         <v>99895</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C71" s="1">
         <v>823</v>
@@ -3166,13 +2894,13 @@
         <v>693</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G71" s="1">
         <v>1180</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -3185,7 +2913,7 @@
         <v>99896</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C72" s="1">
         <v>848</v>
@@ -3197,13 +2925,13 @@
         <v>323</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="G72" s="1">
         <v>698</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -3216,7 +2944,7 @@
         <v>99897</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C73" s="1">
         <v>823</v>
@@ -3228,13 +2956,13 @@
         <v>323</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="G73" s="1">
         <v>1180</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -3247,7 +2975,7 @@
         <v>99898</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C74" s="1">
         <v>823</v>
@@ -3259,13 +2987,13 @@
         <v>362</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="G74" s="1">
         <v>387</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -3278,7 +3006,7 @@
         <v>99899</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C75" s="1">
         <v>828</v>
@@ -3290,13 +3018,13 @@
         <v>361</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G75" s="1">
         <v>387</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
@@ -3309,7 +3037,7 @@
         <v>99900</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C76" s="1">
         <v>823</v>
@@ -3321,13 +3049,13 @@
         <v>690</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G76" s="1">
         <v>849</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
@@ -3340,7 +3068,7 @@
         <v>99901</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C77" s="1">
         <v>848</v>
@@ -3352,13 +3080,13 @@
         <v>795</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G77" s="1">
         <v>825</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
@@ -3371,7 +3099,7 @@
         <v>99903</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C78" s="1">
         <v>823</v>
@@ -3383,13 +3111,13 @@
         <v>693</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G78" s="1">
         <v>1179</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
@@ -3402,7 +3130,7 @@
         <v>99904</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C79" s="1">
         <v>863</v>
@@ -3414,13 +3142,13 @@
         <v>663</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G79" s="1">
         <v>649</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
@@ -3433,7 +3161,7 @@
         <v>99905</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C80" s="1">
         <v>830</v>
@@ -3445,13 +3173,13 @@
         <v>323</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G80" s="1">
         <v>712</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
@@ -3464,7 +3192,7 @@
         <v>99907</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C81" s="1">
         <v>815</v>
@@ -3476,13 +3204,13 @@
         <v>396</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G81" s="1">
         <v>377</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
@@ -3495,7 +3223,7 @@
         <v>99909</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C82" s="1">
         <v>841</v>
@@ -3507,13 +3235,13 @@
         <v>323</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="G82" s="1">
         <v>541</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
@@ -3526,7 +3254,7 @@
         <v>99910</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C83" s="1">
         <v>379</v>
@@ -3538,13 +3266,13 @@
         <v>398</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G83" s="1">
         <v>485</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
@@ -3557,7 +3285,7 @@
         <v>99911</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C84" s="1">
         <v>823</v>
@@ -3569,13 +3297,13 @@
         <v>665</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G84" s="1">
         <v>645</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
@@ -3588,7 +3316,7 @@
         <v>99913</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C85" s="1">
         <v>823</v>
@@ -3600,13 +3328,13 @@
         <v>1078</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G85" s="1">
         <v>876</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
@@ -3619,7 +3347,7 @@
         <v>99916</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C86" s="1">
         <v>817</v>
@@ -3631,13 +3359,13 @@
         <v>665</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G86" s="1">
         <v>643</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
@@ -3650,7 +3378,7 @@
         <v>99920</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C87" s="1">
         <v>827</v>
@@ -3662,13 +3390,13 @@
         <v>323</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G87" s="1">
         <v>648</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
@@ -3681,7 +3409,7 @@
         <v>99921</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1">
         <v>823</v>
@@ -3693,13 +3421,13 @@
         <v>562</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G88" s="1">
         <v>516</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
@@ -3712,7 +3440,7 @@
         <v>99922</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C89" s="1">
         <v>817</v>
@@ -3724,13 +3452,13 @@
         <v>323</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="G89" s="1">
         <v>381</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
@@ -3743,7 +3471,7 @@
         <v>99923</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C90" s="1">
         <v>827</v>
@@ -3755,13 +3483,13 @@
         <v>561</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G90" s="1">
         <v>450</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
@@ -3774,7 +3502,7 @@
         <v>99924</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C91" s="1">
         <v>823</v>
@@ -3786,13 +3514,13 @@
         <v>362</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="G91" s="1">
         <v>387</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
@@ -3805,7 +3533,7 @@
         <v>99925</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C92" s="1">
         <v>823</v>
@@ -3817,13 +3545,13 @@
         <v>323</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="G92" s="1">
         <v>704</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
@@ -3836,7 +3564,7 @@
         <v>99926</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C93" s="1">
         <v>823</v>
@@ -3848,13 +3576,13 @@
         <v>323</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="G93" s="1">
         <v>648</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
@@ -3867,7 +3595,7 @@
         <v>99927</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C94" s="1">
         <v>823</v>
@@ -3879,13 +3607,13 @@
         <v>323</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G94" s="1">
         <v>1098</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
@@ -3898,7 +3626,7 @@
         <v>99928</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C95" s="1">
         <v>823</v>
@@ -3910,13 +3638,13 @@
         <v>323</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G95" s="1">
         <v>645</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
@@ -3929,7 +3657,7 @@
         <v>99929</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C96" s="1">
         <v>377</v>
@@ -3941,13 +3669,13 @@
         <v>398</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G96" s="1">
         <v>485</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
@@ -3960,7 +3688,7 @@
         <v>99930</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C97" s="1">
         <v>823</v>
@@ -3972,13 +3700,13 @@
         <v>665</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G97" s="1">
         <v>1317</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
@@ -3991,7 +3719,7 @@
         <v>99931</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C98" s="1">
         <v>842</v>
@@ -4003,13 +3731,13 @@
         <v>553</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G98" s="1">
         <v>564</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
@@ -4022,7 +3750,7 @@
         <v>99932</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C99" s="1">
         <v>371</v>
@@ -4034,13 +3762,13 @@
         <v>398</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G99" s="1">
         <v>485</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
@@ -4053,7 +3781,7 @@
         <v>99933</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C100" s="1">
         <v>824</v>
@@ -4065,13 +3793,13 @@
         <v>1144</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G100" s="1">
         <v>1098</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
@@ -4084,7 +3812,7 @@
         <v>99934</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C101" s="1">
         <v>828</v>
@@ -4096,13 +3824,13 @@
         <v>553</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G101" s="1">
         <v>703</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
@@ -4115,7 +3843,7 @@
         <v>99935</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C102" s="1">
         <v>377</v>
@@ -4127,13 +3855,13 @@
         <v>398</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G102" s="1">
         <v>494</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
@@ -4146,7 +3874,7 @@
         <v>99936</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C103" s="1">
         <v>827</v>
@@ -4158,13 +3886,13 @@
         <v>323</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="G103" s="1">
         <v>843</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
@@ -4177,7 +3905,7 @@
         <v>99937</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C104" s="1">
         <v>823</v>
@@ -4189,13 +3917,13 @@
         <v>664</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G104" s="1">
         <v>646</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
@@ -4208,7 +3936,7 @@
         <v>99939</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C105" s="1">
         <v>823</v>
@@ -4220,13 +3948,13 @@
         <v>664</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G105" s="1">
         <v>647</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
@@ -4239,7 +3967,7 @@
         <v>99940</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C106" s="1">
         <v>823</v>
@@ -4251,13 +3979,13 @@
         <v>665</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G106" s="1">
         <v>1317</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
@@ -4270,7 +3998,7 @@
         <v>99941</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C107" s="1">
         <v>823</v>
@@ -4282,13 +4010,13 @@
         <v>323</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G107" s="1">
         <v>1317</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
@@ -4301,7 +4029,7 @@
         <v>99942</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C108" s="1">
         <v>842</v>
@@ -4313,13 +4041,13 @@
         <v>397</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G108" s="1">
         <v>555</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
@@ -4332,7 +4060,7 @@
         <v>99943</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C109" s="1">
         <v>823</v>
@@ -4344,13 +4072,13 @@
         <v>323</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="G109" s="1">
         <v>379</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
@@ -4363,7 +4091,7 @@
         <v>99945</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C110" s="1">
         <v>816</v>
@@ -4375,13 +4103,13 @@
         <v>323</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="G110" s="1">
         <v>527</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
@@ -4394,7 +4122,7 @@
         <v>99946</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C111" s="1">
         <v>823</v>
@@ -4406,13 +4134,13 @@
         <v>663</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G111" s="1">
         <v>1317</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L111" s="1"/>
       <c r="M111" s="1"/>
@@ -4425,7 +4153,7 @@
         <v>99947</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C112" s="1">
         <v>842</v>
@@ -4437,13 +4165,13 @@
         <v>323</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G112" s="1">
         <v>701</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
@@ -4456,7 +4184,7 @@
         <v>99948</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C113" s="1">
         <v>377</v>
@@ -4468,13 +4196,13 @@
         <v>398</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G113" s="1">
         <v>494</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
@@ -4487,7 +4215,7 @@
         <v>99949</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C114" s="1">
         <v>378</v>
@@ -4499,13 +4227,13 @@
         <v>398</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G114" s="1">
         <v>485</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
@@ -4518,7 +4246,7 @@
         <v>99950</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C115" s="1">
         <v>824</v>
@@ -4530,13 +4258,13 @@
         <v>1144</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G115" s="1">
         <v>1098</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
@@ -4549,7 +4277,7 @@
         <v>99951</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C116" s="1">
         <v>378</v>
@@ -4561,13 +4289,13 @@
         <v>398</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G116" s="1">
         <v>494</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
@@ -4580,7 +4308,7 @@
         <v>99952</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C117" s="1">
         <v>371</v>
@@ -4592,13 +4320,13 @@
         <v>398</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G117" s="1">
         <v>494</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
@@ -4611,7 +4339,7 @@
         <v>99953</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C118" s="1">
         <v>842</v>
@@ -4623,13 +4351,13 @@
         <v>397</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G118" s="1">
         <v>872</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
@@ -4642,7 +4370,7 @@
         <v>99954</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C119" s="1">
         <v>823</v>
@@ -4654,13 +4382,13 @@
         <v>323</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="G119" s="1">
         <v>645</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
@@ -4673,7 +4401,7 @@
         <v>99955</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C120" s="1">
         <v>826</v>
@@ -4685,13 +4413,13 @@
         <v>1096</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G120" s="1">
         <v>1210</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
@@ -4704,7 +4432,7 @@
         <v>99956</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C121" s="1">
         <v>823</v>
@@ -4716,13 +4444,13 @@
         <v>11</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G121" s="1">
         <v>732</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
@@ -4735,7 +4463,7 @@
         <v>99957</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C122" s="1">
         <v>823</v>
@@ -4747,13 +4475,13 @@
         <v>795</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G122" s="1">
         <v>832</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
@@ -4766,7 +4494,7 @@
         <v>99958</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C123" s="1">
         <v>827</v>
@@ -4778,13 +4506,13 @@
         <v>323</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="G123" s="1">
         <v>876</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
@@ -4797,7 +4525,7 @@
         <v>99960</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C124" s="1">
         <v>823</v>
@@ -4809,13 +4537,13 @@
         <v>391</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G124" s="1">
         <v>516</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
@@ -4828,7 +4556,7 @@
         <v>99961</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C125" s="1">
         <v>820</v>
@@ -4840,13 +4568,13 @@
         <v>803</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G125" s="1">
         <v>835</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
@@ -4859,7 +4587,7 @@
         <v>99962</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C126" s="1">
         <v>823</v>
@@ -4871,13 +4599,13 @@
         <v>392</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G126" s="1">
         <v>516</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
@@ -4890,7 +4618,7 @@
         <v>99963</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C127" s="1">
         <v>377</v>
@@ -4902,13 +4630,13 @@
         <v>398</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G127" s="1">
         <v>494</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
@@ -4921,7 +4649,7 @@
         <v>99964</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C128" s="1">
         <v>817</v>
@@ -4933,13 +4661,13 @@
         <v>1144</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G128" s="1">
         <v>1098</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
@@ -4952,7 +4680,7 @@
         <v>99965</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C129" s="1">
         <v>377</v>
@@ -4964,13 +4692,13 @@
         <v>323</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="G129" s="1">
         <v>494</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
@@ -4983,7 +4711,7 @@
         <v>99966</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C130" s="1">
         <v>842</v>
@@ -4995,13 +4723,13 @@
         <v>323</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="G130" s="1">
         <v>377</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
@@ -5014,7 +4742,7 @@
         <v>99967</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C131" s="1">
         <v>820</v>
@@ -5026,13 +4754,13 @@
         <v>803</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G131" s="1">
         <v>835</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
@@ -5045,7 +4773,7 @@
         <v>99968</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C132" s="1">
         <v>815</v>
@@ -5057,13 +4785,13 @@
         <v>323</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G132" s="1">
         <v>700</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
@@ -5076,7 +4804,7 @@
         <v>99969</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C133" s="1">
         <v>819</v>
@@ -5088,13 +4816,13 @@
         <v>663</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G133" s="1">
         <v>1316</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
@@ -5107,7 +4835,7 @@
         <v>99970</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C134" s="1">
         <v>823</v>
@@ -5119,13 +4847,13 @@
         <v>403</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="G134" s="1">
         <v>450</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
@@ -5138,7 +4866,7 @@
         <v>99971</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C135" s="1">
         <v>848</v>
@@ -5150,13 +4878,13 @@
         <v>323</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="G135" s="1">
         <v>825</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
@@ -5169,7 +4897,7 @@
         <v>99972</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C136" s="1">
         <v>827</v>
@@ -5181,13 +4909,13 @@
         <v>323</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G136" s="1">
         <v>387</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
@@ -5200,7 +4928,7 @@
         <v>99973</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C137" s="1">
         <v>847</v>
@@ -5212,13 +4940,13 @@
         <v>414</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="G137" s="1">
         <v>727</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
@@ -5231,7 +4959,7 @@
         <v>99974</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C138" s="1">
         <v>820</v>
@@ -5243,13 +4971,13 @@
         <v>1096</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G138" s="1">
         <v>541</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
@@ -5262,7 +4990,7 @@
         <v>99975</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C139" s="1">
         <v>824</v>
@@ -5274,13 +5002,13 @@
         <v>1144</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G139" s="1">
         <v>1098</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
@@ -5293,7 +5021,7 @@
         <v>99976</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C140" s="1">
         <v>828</v>
@@ -5305,13 +5033,13 @@
         <v>323</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G140" s="1">
         <v>378</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="141" spans="1:16">
@@ -5319,7 +5047,7 @@
         <v>99977</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C141" s="1">
         <v>816</v>
@@ -5331,13 +5059,13 @@
         <v>323</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G141" s="1">
         <v>703</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="142" spans="1:16">
@@ -5345,7 +5073,7 @@
         <v>99979</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C142" s="1">
         <v>863</v>
@@ -5357,13 +5085,13 @@
         <v>803</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G142" s="1">
         <v>550</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="143" spans="1:16">
@@ -5371,7 +5099,7 @@
         <v>99980</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C143" s="1">
         <v>827</v>
@@ -5383,13 +5111,13 @@
         <v>323</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="G143" s="1">
         <v>387</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="144" spans="1:16">
@@ -5397,7 +5125,7 @@
         <v>99981</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C144" s="1">
         <v>830</v>
@@ -5409,13 +5137,13 @@
         <v>323</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="G144" s="1">
         <v>712</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5423,7 +5151,7 @@
         <v>99982</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C145" s="1">
         <v>848</v>
@@ -5435,13 +5163,13 @@
         <v>323</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="G145" s="1">
         <v>1175</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5449,7 +5177,7 @@
         <v>99983</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C146" s="1">
         <v>848</v>
@@ -5461,13 +5189,13 @@
         <v>803</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G146" s="1">
         <v>825</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5475,7 +5203,7 @@
         <v>99984</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C147" s="1">
         <v>823</v>
@@ -5487,13 +5215,13 @@
         <v>665</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G147" s="1">
         <v>648</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5501,7 +5229,7 @@
         <v>99985</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C148" s="1">
         <v>828</v>
@@ -5513,13 +5241,13 @@
         <v>323</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="G148" s="1">
         <v>511</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5527,7 +5255,7 @@
         <v>99986</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C149" s="1">
         <v>830</v>
@@ -5539,13 +5267,13 @@
         <v>466</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G149" s="1">
         <v>383</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5553,7 +5281,7 @@
         <v>99987</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C150" s="1">
         <v>817</v>
@@ -5565,13 +5293,13 @@
         <v>1097</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G150" s="1">
         <v>650</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5579,7 +5307,7 @@
         <v>99988</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C151" s="1">
         <v>830</v>
@@ -5591,13 +5319,13 @@
         <v>323</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="G151" s="1">
         <v>358</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5605,7 +5333,7 @@
         <v>99990</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C152" s="1">
         <v>823</v>
@@ -5617,13 +5345,13 @@
         <v>392</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G152" s="1">
         <v>704</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5631,7 +5359,7 @@
         <v>99991</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C153" s="1">
         <v>823</v>
@@ -5643,13 +5371,13 @@
         <v>323</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="G153" s="1">
         <v>387</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5657,7 +5385,7 @@
         <v>99992</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C154" s="1">
         <v>823</v>
@@ -5669,13 +5397,13 @@
         <v>412</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G154" s="1">
         <v>388</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5683,7 +5411,7 @@
         <v>99993</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C155" s="1">
         <v>823</v>
@@ -5695,13 +5423,13 @@
         <v>407</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="G155" s="1">
         <v>388</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5709,7 +5437,7 @@
         <v>99994</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C156" s="1">
         <v>819</v>
@@ -5721,13 +5449,13 @@
         <v>466</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G156" s="1">
         <v>704</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5735,7 +5463,7 @@
         <v>99995</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C157" s="1">
         <v>848</v>
@@ -5747,13 +5475,13 @@
         <v>802</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G157" s="1">
         <v>825</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5761,7 +5489,7 @@
         <v>99996</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C158" s="1">
         <v>820</v>
@@ -5773,13 +5501,13 @@
         <v>392</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G158" s="1">
         <v>874</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5787,7 +5515,7 @@
         <v>99997</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C159" s="1">
         <v>823</v>
@@ -5799,13 +5527,13 @@
         <v>328</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G159" s="1">
         <v>876</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5813,7 +5541,7 @@
         <v>99998</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C160" s="1">
         <v>823</v>
@@ -5825,13 +5553,13 @@
         <v>399</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="G160" s="1">
         <v>381</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5839,7 +5567,7 @@
         <v>99999</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C161" s="1">
         <v>377</v>
@@ -5851,13 +5579,13 @@
         <v>398</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G161" s="1">
         <v>494</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5865,7 +5593,7 @@
         <v>100000</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C162" s="1">
         <v>378</v>
@@ -5877,13 +5605,13 @@
         <v>398</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G162" s="1">
         <v>494</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5891,7 +5619,7 @@
         <v>100001</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C163" s="1">
         <v>371</v>
@@ -5903,13 +5631,13 @@
         <v>398</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G163" s="1">
         <v>494</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -5917,7 +5645,7 @@
         <v>100004</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C164" s="1">
         <v>377</v>
@@ -5929,13 +5657,13 @@
         <v>398</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G164" s="1">
         <v>494</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -5943,7 +5671,7 @@
         <v>100005</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C165" s="1">
         <v>377</v>
@@ -5955,13 +5683,13 @@
         <v>398</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G165" s="1">
         <v>485</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -5969,7 +5697,7 @@
         <v>100006</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C166" s="1">
         <v>817</v>
@@ -5981,13 +5709,13 @@
         <v>323</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="G166" s="1">
         <v>380</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -5995,7 +5723,7 @@
         <v>100007</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C167" s="1">
         <v>817</v>
@@ -6007,13 +5735,13 @@
         <v>360</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G167" s="1">
         <v>703</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6021,7 +5749,7 @@
         <v>100008</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C168" s="1">
         <v>842</v>
@@ -6033,13 +5761,13 @@
         <v>323</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G168" s="1">
         <v>450</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>